<commit_message>
Bug fix, output image and output table headers.
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/Score_cfg.xlsx
+++ b/ConfigurationFiles/Score_cfg.xlsx
@@ -27,24 +27,12 @@
     <t>Type</t>
   </si>
   <si>
-    <t>M-sn1</t>
-  </si>
-  <si>
     <t>sn1</t>
   </si>
   <si>
     <t>sn2</t>
   </si>
   <si>
-    <t>M-sn2</t>
-  </si>
-  <si>
-    <t>M-(sn1-H2O)</t>
-  </si>
-  <si>
-    <t>M-(sn2-H2O)</t>
-  </si>
-  <si>
     <t>FA</t>
   </si>
   <si>
@@ -55,6 +43,18 @@
   </si>
   <si>
     <t>[M+HCOO]-</t>
+  </si>
+  <si>
+    <t>[M-H]-sn2</t>
+  </si>
+  <si>
+    <t>[M-H]-sn1</t>
+  </si>
+  <si>
+    <t>[M-H]-sn1-H2O</t>
+  </si>
+  <si>
+    <t>[M-H]-sn2-H2O</t>
   </si>
 </sst>
 </file>
@@ -427,21 +427,21 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>25</v>
@@ -461,7 +461,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>25</v>
@@ -481,7 +481,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>15</v>
@@ -501,7 +501,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>15</v>
@@ -521,7 +521,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -561,5 +561,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
hot fix for MS1 centroid Thermo .mzML files in Shotgun mode
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/Score_cfg.xlsx
+++ b/ConfigurationFiles/Score_cfg.xlsx
@@ -409,7 +409,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +496,7 @@
         <v>-1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -516,7 +516,7 @@
         <v>-1</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -536,7 +536,7 @@
         <v>-1</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -556,7 +556,7 @@
         <v>-1</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Isotope score functional. Rank score under development. Score configuration table columns updated.
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/Score_cfg.xlsx
+++ b/ConfigurationFiles/Score_cfg.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Weight</t>
   </si>
@@ -27,34 +27,25 @@
     <t>Type</t>
   </si>
   <si>
-    <t>sn1</t>
-  </si>
-  <si>
-    <t>sn2</t>
-  </si>
-  <si>
-    <t>FA</t>
-  </si>
-  <si>
-    <t>H2O</t>
-  </si>
-  <si>
-    <t>[M-H]-</t>
-  </si>
-  <si>
-    <t>[M+HCOO]-</t>
-  </si>
-  <si>
-    <t>[M-H]-sn2</t>
-  </si>
-  <si>
-    <t>[M-H]-sn1</t>
-  </si>
-  <si>
-    <t>[M-H]-sn1-H2O</t>
-  </si>
-  <si>
-    <t>[M-H]-sn2-H2O</t>
+    <t>SN1_[FA-H]-</t>
+  </si>
+  <si>
+    <t>SN2_[FA-H]-</t>
+  </si>
+  <si>
+    <t>[LPL(SN1)-H2O-H]-</t>
+  </si>
+  <si>
+    <t>[LPL(SN2)-H2O-H]-</t>
+  </si>
+  <si>
+    <t>[LPL(SN1)-H]-</t>
+  </si>
+  <si>
+    <t>[LPL(SN2)-H]-</t>
+  </si>
+  <si>
+    <t>Group</t>
   </si>
 </sst>
 </file>
@@ -406,20 +397,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -427,19 +416,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -447,19 +427,10 @@
         <v>25</v>
       </c>
       <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -467,96 +438,51 @@
         <v>25</v>
       </c>
       <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>15</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>-1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>15</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>-1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>-1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
       <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>-1</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>